<commit_message>
Added Updated Base64 Image Ref.xlsx File
</commit_message>
<xml_diff>
--- a/Base64 Image Ref.xlsx
+++ b/Base64 Image Ref.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F910849-CED8-4A2F-915F-046D4C3FD778}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D7A329D-536D-42CE-99FC-03AD87BE3F43}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11310" tabRatio="813" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11310" tabRatio="813" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Active Directory (16x16)" sheetId="3" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="122">
   <si>
     <t>Control Panel</t>
   </si>
@@ -381,6 +381,18 @@
   </si>
   <si>
     <t>iVBORw0KGgoAAAANSUhEUgAAABAAAAAQCAYAAAAf8/9hAAAAAXNSR0IArs4c6QAAAARnQU1BAACxjwv8YQUAAAAJcEhZcwAADsIAAA7CARUoSoAAAALYSURBVDhPfZPPTxNREMc/uy2l8ksBES3RSEmaJpoSEwV/JBr1gBhjosSDESWiF+PRo/+BelDjwZPhoqjRRBNPJiocrRGlIm0FkQQobalQiq0tZfc5uzQxeHCSefNm9s3Md36splAqPPKJv2RZSjdliGZfLKsI0YQDu/bZ3y3SRkeG1IePoZIKuqahO3R0XcftLhfpwCm6w7kqGzauZzY+T0fnCfu90z6FenqqoaYRHJvEupmr16rpkjepDGRNKKzA/MIKR+uDGIYYSqSXJPqGIriyUJeTAGlS0wW8dRDwQFszHN0BB3zWc4VhrgmgBKZG81bx1yRdXlhbYmg0w8iYYiYJ49MwITyVXO2FsWKU3CWAQkOTuj1bnFS4JXtuDswEidgM4WiGuWSe2MwyszElLHX8g8CJMnG5XOQLBdZXm2SyOUyjjMKSTmRsgd/pCHOzwyykxjBlAj+/eaitrS+5l3rgkI7H45JdM2QKeUGQo7icocH9hhpXlLNnDnL3zk3u3b1FR8dx8dB48viJ5YpTCQJrbFNRge4qg2ULZhqfv8jm+gouXemlyiUTErLqr2wuw1vZxPe30wwODKJ9CQWt7ZCsctprZa2O4tnzV3TKrGta1tFQ2UhDRSPD8SFO9u/jtP8cp6ouEnwfRN8Z2MNiJsv84hKp1CLJZNpelMnJKfx+P/0jDzjSFyC+FKfr6SGaqrdxff8NvM1eIpGIDcta1DU8Pj6uuru7VSqVUsViUe2+v01dftGlstmsarldqa6+PKcmfkyo3t7eVdB2gUKJeIJ0Oi1zztLf/5yOY528yj3k8dcHDJ4PU+vaSOJXjHLdTfhzhOFQiDUBBt69tmU+XyA8GpWe6Bw8vZdyxzq2Vm2352+smJimQV9fH+3t7WsD/EuPHj4iFovR2hrA622Rf8BAyiMUGsbjaeJCz4X/B7Bo4N0AwWCQaDRq6z6fj7a2Ng4fOSwa/AG4ymS9w/YvnQAAAABJRU5ErkJggg==</t>
+  </si>
+  <si>
+    <t>Arrow-Up</t>
+  </si>
+  <si>
+    <t>iVBORw0KGgoAAAANSUhEUgAAABEAAAARCAMAAAAMs7fIAAAABGdBTUEAALGPC/xhBQAAACBjSFJNAAB6JgAAgIQAAPoAAACA6AAAdTAAAOpgAAA6mAAAF3CculE8AAAB+1BMVEUAAADJz+K+x/CgremQn+WkserByvDe4fCWpOS1v+rT2fLt7/j8/P3u8frV2vO2wOyhruaksOTT2e79/f3+/v7X3PKpteajr+H9/v38/v3i5vStuOWRn9nR2Ov2+ff1+Pf1+Pb19/b19/X09/XS2eyptOGuuN/u8O/s8O7r7+zq7uzp7evo7Ovo7Onp7erp7ezr7u25wuO4weLAx93k5+Xj6Obh5+Pg5eLe4+Dc4t9PaNbc4d7d4uDf4+Hg5OLh5eTCyeaUo9DM097e4t/Z4N1CXLrX29jY3drZ3tzO1dyyvN2AkMPb4N/Q19PZ39zW3dgwSpLU2tfU2tbY3trL09ClsNWVocnJz9W+xsHa39zX3NgeN2nT2tbS2tS9xsips9O0vda2v9C/yMPJz8zR1tTN1NHM1NDCysfAyNW0vtaeqcXHzcm0vrm8xMC+xsO/xsO/x8O/yMS8xMHFzMqvu7a1vtOKmLm8xM/P1tTHzsu4wby5wr23wbu2wLq1v7m2v7q5w767xMHDzNWUob+Uob3K0dfi5eTX3tvT2dbKz8zGzcnHzsnIzsvR2NTN09ujrsWYo7zGy9fs7uzs8u7p8ezp7+vq8u3o7enLz9mfqsGGlLClr8LCydTd5OTu9fDg5+fGzdeps8WFk6+gqryLmLB+jKiJlq+dqLv///+AEltLAAAAAXRSTlMAQObYZgAAAAFiS0dEqFAINpIAAAAJcEhZcwAADsMAAA7DAcdvqGQAAAAHdElNRQflAwQJIjtb91mdAAAA/0lEQVQY02NgAAFGJmYWVjZGBhhg5+Dk4ubh5eMXYIcKCAoJi4CBqBhYiF2cXQIIJCUlJSSkpEFCMrJy8gqKSspAoKigogo0VE1dQ1NLW0dXV0dPX8vAkJHByNjE1MzcwtLK2tLG1s6e0YHB0cnZ2sXFxdXV1cXFzd3D04vB28fXz98/AAT8A4OCQ0IZwsIjIqOiISAmNiYuniEhMSk5BQpS09IzMhkYs7JzcvPyCwoLC/KKiktKgV4pK6+orKquqa2rr25obGoGubmlta29o7Oruye7t68f4o0JEydNnjJ16rTpM2bCvDpr9py58+YvWLiIHR4ejIuXLF22HBI+AOZ3RVSg/ukZAAAAJXRFWHRkYXRlOmNyZWF0ZQAyMDIxLTAzLTA0VDA5OjM0OjUxKzAwOjAwldgBXwAAACV0RVh0ZGF0ZTptb2RpZnkAMjAyMS0wMy0wNFQwOTozNDo1MSswMDowMOSFueMAAAAASUVORK5CYII=</t>
+  </si>
+  <si>
+    <t>Arrow-Down</t>
+  </si>
+  <si>
+    <t>iVBORw0KGgoAAAANSUhEUgAAABEAAAARCAMAAAAMs7fIAAAABGdBTUEAALGPC/xhBQAAACBjSFJNAAB6JgAAgIQAAPoAAACA6AAAdTAAAOpgAAA6mAAAF3CculE8AAACB1BMVEUAAADJz+K+x/CgremQn+WkserByvDe4fCWpOS1v+rT2fLt7/j8/P3u8frV2vO2wOyhruaksOTT2e79/f3+/v7X3PKpteajr+H9/v38/v3i5vStuOWRn9nR2Ov2+ff1+Pf1+Pb19/b19/X09/XS2eyptOGuuN/u8O/s8O7r7+zq7uzp7evo7Ovo7Onp7erp7ezr7u25wuO4weLAx93k5+Xj6Obh5+Pg5eLe4+Dc4t/c4d7d4uDf4+Hg5OLh5eTCyeaUo9DM097e4t/Z4N1PaNbX29jY3drZ3tzO1dyyvN2AkMPb4N/Q19PZ39zW3djU29dCXLrS2NbU2tfU2tbY3trL09ClsNWVocnJz9W+xsHa39zX3NjT2tYwSpLT2tXS2tS9xsips9O0vda2v9C/yMPJz8zR1tTN1NEeN2nN1NDM1NDCysfAyNW0vtaeqcXHzcm0vrm8xMC+xsO/xsO/x8O/yMS8xMHFzMqvu7a1vtOKmLm8xM/P1tTHzsu4wby5wr23wbu2wLq1v7m2v7q5w767xMHDzNWUob+Uob3K0dfi5eTX3tvT2dbKz8zGzcnHzsnIzsvR2NTN09ujrsWYo7zGy9fs7uzs8u7p8ezp7+vq8u3o7enLz9mfqsGGlLClr8LCydTd5OTu9fDg5+fGzdeps8WFk6+gqryLmLB+jKiJlq+dqLv////3st2kAAAAAXRSTlMAQObYZgAAAAFiS0dErFdl8osAAAAJcEhZcwAADsMAAA7DAcdvqGQAAAAHdElNRQflAwMSMRVramHoAAABBUlEQVQY02NgAAFGJmYWVjZGBhhg5+Dk4ubh5eMXYIcKCAoJi4CBqBhYiF2cXQIIJCUlJSSkpEFCMrJy8gqKSspAoKigogo0VE1dQ1NLW0dXV0dPX8vAkJHByNjE1MzcwtLKytLaxtaO0Z7BwdHJytkFAlzd3D08Gby8fXz9/ANAIDAoOCQ0jCE8IjIqOjgmNjY2Li4mPiYhkSEpOSU1LT09PSMzMzM9Kzsnl4ExL7+gsKi4pLS0pKisvKIS6JWq6prauvqGxqbm+pbWtnaQmzs6u7p7evv6J+RPnDQZ4o0pU6dNnzFz5qzZc+bCvDpv/oKFixYvWbqMHR4ejMtXrFy1GhI+AD9FRpvxXGkwAAAAJXRFWHRkYXRlOmNyZWF0ZQAyMDIxLTAzLTAzVDE4OjQ5OjA2KzAwOjAweTpvAAAAACV0RVh0ZGF0ZTptb2RpZnkAMjAyMS0wMy0wM1QxODo0OTowNiswMDowMAhn17wAAAAASUVORK5CYII=</t>
   </si>
 </sst>
 </file>
@@ -3001,6 +3013,128 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EDE07E76-6A74-445A-986C-EAA2911317BA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1895475" y="400050"/>
+          <a:ext cx="161925" cy="161925"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{94C2A342-0CAE-4587-83E1-BD1194374000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1895475" y="590550"/>
+          <a:ext cx="161925" cy="161925"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4373,7 +4507,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B490FD4-615E-4B04-A7F8-FFA74CBC5766}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
@@ -4831,7 +4965,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4869,16 +5003,28 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
+      <c r="A3" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>51</v>
+      </c>
       <c r="C3" s="6"/>
-      <c r="D3" s="12"/>
+      <c r="D3" s="12" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
+      <c r="A4" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>51</v>
+      </c>
       <c r="C4" s="6"/>
-      <c r="D4" s="12"/>
+      <c r="D4" s="12" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
@@ -4924,7 +5070,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>

</xml_diff>